<commit_message>
[CCORDERO] Resnet152 analysis added to graphs comparison
</commit_message>
<xml_diff>
--- a/presicion_analisis_Resnet152.xlsx
+++ b/presicion_analisis_Resnet152.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DB99D5-EF03-472B-BF05-2EB226E78EC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B1D2FE-5923-4C39-BA65-7B1423930889}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6Resnet1520.00004" sheetId="1" r:id="rId1"/>
@@ -351,17 +351,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>226072</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>58156</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>791985</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>163489</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57DA9076-B0E8-40DD-994A-D80EC2E74AB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8242C38-33E5-4CAE-AF48-CA2CDD911974}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -378,7 +378,51 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4980952" cy="7190476"/>
+          <a:ext cx="3961905" cy="2723809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28076</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>106347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21151F86-7A65-46E2-B30E-955A8328C178}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4754880" y="0"/>
+          <a:ext cx="3990476" cy="2666667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -863,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CB1C0E-36A0-4ECC-8690-FEF5C84C5B3D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,7 +922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1616795-5C10-47C4-B0FC-EA6BE55562CC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[CCORDERO] no reduce on plateau in Resnet152
</commit_message>
<xml_diff>
--- a/presicion_analisis_Resnet152.xlsx
+++ b/presicion_analisis_Resnet152.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CARLOS CORDERO\Desktop\ToG_pretrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B1D2FE-5923-4C39-BA65-7B1423930889}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B3884C-C02B-4F46-80F4-3897B804114C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{ABC54316-D9C0-4881-9B1E-066589C50761}"/>
   </bookViews>
   <sheets>
     <sheet name="6Resnet1520.00004" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="6Resnet1520.00008" sheetId="12" r:id="rId3"/>
     <sheet name="6Resnet1520.0001" sheetId="13" r:id="rId4"/>
     <sheet name="6Resnet1520.00007" sheetId="14" r:id="rId5"/>
-    <sheet name="63Resnet1520.00008" sheetId="15" r:id="rId6"/>
-    <sheet name="6Resnet1520.00008_ReduceLR" sheetId="16" r:id="rId7"/>
+    <sheet name="6Resnet1520.00008_ReduceLR" sheetId="16" r:id="rId6"/>
+    <sheet name="63Resnet1520.00008_ReduceLR" sheetId="15" r:id="rId7"/>
+    <sheet name="63Resnet1520.00008" sheetId="17" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -342,6 +343,99 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>199505</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>56800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B768E369-E899-49D7-A099-7BD2418DFA94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4161905" cy="2800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104267</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>173013</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95D48AD-723B-4764-9D24-7529CD4641AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4754880" y="0"/>
+          <a:ext cx="4066667" cy="2733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -434,7 +528,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -445,16 +539,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>199505</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>56800</xdr:rowOff>
+      <xdr:colOff>647125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>18663</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B768E369-E899-49D7-A099-7BD2418DFA94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3BAC99-4A84-447E-B190-F616BFA1B6EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -471,7 +565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4161905" cy="2800000"/>
+          <a:ext cx="4600000" cy="3095238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -482,23 +576,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>104267</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>173013</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>456649</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28187</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E95D48AD-723B-4764-9D24-7529CD4641AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AB4857E-C40C-4DF5-93D6-8092798AA7F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -514,8 +608,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4754880" y="0"/>
-          <a:ext cx="4066667" cy="2733333"/>
+          <a:off x="5534025" y="0"/>
+          <a:ext cx="4409524" cy="3104762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -904,21 +998,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CB1C0E-36A0-4ECC-8690-FEF5C84C5B3D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1616795-5C10-47C4-B0FC-EA6BE55562CC}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -931,4 +1010,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CB1C0E-36A0-4ECC-8690-FEF5C84C5B3D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CCA5F7-3B33-45D2-8437-030C12BA7427}">
+  <dimension ref="E21:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>